<commit_message>
adding nonFP_species_richness to transformations
</commit_message>
<xml_diff>
--- a/GLM/glm best transformations.xlsx
+++ b/GLM/glm best transformations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>surfacearea_ha</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>nonFP_species_richness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actually a power + 1 (added 1, then did a power transformation) </t>
   </si>
 </sst>
 </file>
@@ -468,16 +474,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A2:A20"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -886,6 +892,29 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.78719160311813596</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-0.61583965622978298</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-5.0038249999999999E-2</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.35095150000000003</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Too many missed commits!!!
</commit_message>
<xml_diff>
--- a/GLM/glm best transformations.xlsx
+++ b/GLM/glm best transformations.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="10110"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="10110" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="skewness" sheetId="1" r:id="rId1"/>
+    <sheet name="skewness-8-15-2014" sheetId="1" r:id="rId1"/>
+    <sheet name="skewness-12-8-2014" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>surfacearea_ha</t>
   </si>
@@ -101,13 +102,16 @@
   </si>
   <si>
     <t xml:space="preserve">Actually a power + 1 (added 1, then did a power transformation) </t>
+  </si>
+  <si>
+    <t>nearest_any_FP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -125,6 +129,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -164,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -173,6 +183,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
@@ -919,4 +935,447 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2.5550230810309298</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.8239452297867298E-2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-0.70675885031840502</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-6.2061026673663797E-2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.15079021142298701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.5385252326425201</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.81305820523314798</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.54633153115934896</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3.7401477946466199E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>-0.84891169475616801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.54862504771485</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.47702875319704602</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5.1707768232656499E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2.2116706736453901E-3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-2.5437663794861402E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.78531813945735396</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-0.72092019288438203</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8.4722266734366691</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.1784689331381104</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5.7228241189872603E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-2.39674123516274E-3</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-1.54323057984614E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.66233313692425499</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.30884463652887001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.25685259806602201</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-1.47029135857429E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-0.69184525552501297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.2205797603992501</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-0.253837870070731</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-0.27210680378734198</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-1.5456192799464001E-2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.163450962122275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2.7749796416371599</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-0.19439518213762699</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-0.44425177468893301</v>
+      </c>
+      <c r="E9" s="9">
+        <v>8.5215636481767202E-4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.14167748662264401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.7161323300909599</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.35609677204644902</v>
+      </c>
+      <c r="D10" s="5">
+        <v>-0.27315684397842099</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-2.9303743773363401E-4</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.15435806923850701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.83840282405920696</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-0.21162441492678999</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.84994708665888996</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-0.170895828630338</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-0.236661127413685</v>
+      </c>
+      <c r="E12" s="9">
+        <v>6.8713346234863999E-4</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.20804492687753401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.53578995520832895</v>
+      </c>
+      <c r="C13" s="5">
+        <v>-0.14897417257418799</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-0.16027914625415099</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-7.3503719614283897E-3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.20934620240301699</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1.6882487549199701</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-1.14519704621594</v>
+      </c>
+      <c r="D14" s="5">
+        <v>-1.1480176535336</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-1.2050154345292399E-2</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.344699109463947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.41122465049533702</v>
+      </c>
+      <c r="C15" s="5">
+        <v>-1.63133745870889</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-1.6331111787714001</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0.120637543142068</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.61401065110270203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.839637451964512</v>
+      </c>
+      <c r="C16" s="5">
+        <v>-1.6753406824933701</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-1.6798239714754499</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-7.3158416889426398E-2</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.51793007397773705</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.98012547043815501</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-1.49394807810816</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-1.49798715615136</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-9.32997633328497E-2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.51793007397773705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.1547005383792499</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.1547005383792499</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1.4702292871462801</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-1.36667752928391</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-1.38356500939844</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1.9291911050949899E-2</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.26180654206100701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.31394593515389202</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.30552351128672001</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.30532057672822599</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.224762185102307</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-7.6541660139325396</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="3">
+        <v>5.7267382136044098E-2</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>